<commit_message>
order persistence and customer ui
</commit_message>
<xml_diff>
--- a/data/order_list.xlsx
+++ b/data/order_list.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanjanashanmugasundaram/IdeaProjects/SC2002_OOP_FOMS/SC2002_OOP_FOMSApp/data/"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
   <si>
     <t>id</t>
   </si>
@@ -57,12 +57,34 @@
   </si>
   <si>
     <t>payment method</t>
+  </si>
+  <si>
+    <t>T-100</t>
+  </si>
+  <si>
+    <t>NTU</t>
+  </si>
+  <si>
+    <t>Chicken tenders</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>NEW</t>
+  </si>
+  <si>
+    <t>Cash</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -434,7 +456,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D9B652-E5C7-AB48-B074-FB8F261F35A4}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:G8"/>
@@ -442,11 +464,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="40.83203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.83203125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="40.83203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="17.83203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,6 +489,29 @@
       </c>
       <c r="G1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed validateString & checkorderstatus errors
</commit_message>
<xml_diff>
--- a/data/order_list.xlsx
+++ b/data/order_list.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="34">
   <si>
     <t>id</t>
   </si>
@@ -122,6 +122,12 @@
   </si>
   <si>
     <t>Chicken Nugget : spicy</t>
+  </si>
+  <si>
+    <t>Fries, Chicken Nugget</t>
+  </si>
+  <si>
+    <t>Fries : spicy</t>
   </si>
 </sst>
 </file>
@@ -507,7 +513,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D9B652-E5C7-AB48-B074-FB8F261F35A4}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -683,6 +689,29 @@
         <v>26</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
misc changes (refer to doc)
</commit_message>
<xml_diff>
--- a/data/order_list.xlsx
+++ b/data/order_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanjanashanmugasundaram/IdeaProjects/SC2002_OOP_FOMS/SC2002_FOMS/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CF08F0-D590-B347-B04C-F8A868DFB449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2641BA33-D8EB-B548-A722-5C14AEA3A001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="19420" windowHeight="10300" xr2:uid="{0C82953F-FE30-0444-AC4E-BE046C6CD01D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="30">
   <si>
     <t>id</t>
   </si>
@@ -42,12 +42,24 @@
     <t>status</t>
   </si>
   <si>
+    <t>takeaway</t>
+  </si>
+  <si>
+    <t>payment</t>
+  </si>
+  <si>
     <t>T-100</t>
   </si>
   <si>
     <t>NTU</t>
   </si>
   <si>
+    <t>Chicken Tenders</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>true</t>
   </si>
   <si>
@@ -57,91 +69,52 @@
     <t>Cash</t>
   </si>
   <si>
-    <t>T-101</t>
+    <t>D-100</t>
+  </si>
+  <si>
+    <t>Fries</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>PayNow</t>
+  </si>
+  <si>
+    <t>READY</t>
+  </si>
+  <si>
+    <t>CANCELLED</t>
+  </si>
+  <si>
+    <t>D-101</t>
   </si>
   <si>
     <t>JE</t>
   </si>
   <si>
-    <t>COLE SLAW, 3PC set meal</t>
-  </si>
-  <si>
-    <t>COLE SLAW : test</t>
+    <t>Pepsi</t>
   </si>
   <si>
     <t>D-102</t>
   </si>
   <si>
+    <t>3pc Set Meal</t>
+  </si>
+  <si>
+    <t>D-103</t>
+  </si>
+  <si>
+    <t>Cole Slaw</t>
+  </si>
+  <si>
+    <t>D-104</t>
+  </si>
+  <si>
     <t>JP</t>
   </si>
   <si>
-    <t>fries, fries</t>
-  </si>
-  <si>
-    <t>fries : test</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
-    <t>takeaway</t>
-  </si>
-  <si>
-    <t>payment</t>
-  </si>
-  <si>
-    <t>D-100</t>
-  </si>
-  <si>
-    <t>Credit/Debit Card</t>
-  </si>
-  <si>
-    <t>Chicken Nugget, Chicken Tenders, Fries</t>
-  </si>
-  <si>
-    <t>Chicken Tenders : test test, Chicken Tenders : test</t>
-  </si>
-  <si>
-    <t>READY</t>
-  </si>
-  <si>
     <t>Chicken Nugget</t>
-  </si>
-  <si>
-    <t>Chicken Nugget : spicy</t>
-  </si>
-  <si>
-    <t>Fries, Chicken Nugget</t>
-  </si>
-  <si>
-    <t>Fries : spicy</t>
-  </si>
-  <si>
-    <t>Chicken Tenders, Chicken Nugget, Tea</t>
-  </si>
-  <si>
-    <t>Chicken Tenders : curry sauce, Chicken Tenders : bbq sauce</t>
-  </si>
-  <si>
-    <t>PayNow</t>
-  </si>
-  <si>
-    <t>Chicken Nugget, Fries</t>
-  </si>
-  <si>
-    <t>Fries : less salt</t>
-  </si>
-  <si>
-    <t>Chicken Nugget : bbq sauce</t>
-  </si>
-  <si>
-    <t>T-105</t>
-  </si>
-  <si>
-    <t>CANCELLED</t>
-  </si>
-  <si>
-    <t>COMPLETED</t>
   </si>
 </sst>
 </file>
@@ -190,9 +163,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -527,250 +501,224 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D9B652-E5C7-AB48-B074-FB8F261F35A4}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="H15" sqref="A2:H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" style="1" width="10.6640625" collapsed="true"/>
     <col min="3" max="3" customWidth="true" style="1" width="40.83203125" collapsed="true"/>
-    <col min="4" max="6" style="1" width="10.6640625" collapsed="true"/>
+    <col min="4" max="5" style="1" width="10.6640625" collapsed="true"/>
     <col min="7" max="7" customWidth="true" style="1" width="17.83203125" collapsed="true"/>
     <col min="8" max="16384" style="1" width="10.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
         <v>26</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
         <v>27</v>
       </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="G7" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" t="s">
-        <v>32</v>
-      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13" s="2"/>
+      <c r="G13"/>
+      <c r="H13"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="G14"/>
+      <c r="H14"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="G15"/>
+      <c r="H15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>